<commit_message>
Traducciones y correcciones menores preinvoice
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
   <si>
     <t>type</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>invoice_id</t>
+  </si>
+  <si>
+    <t>preinvoice</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
   <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,9 +928,48 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>